<commit_message>
updated plotting scripts to increase font size and visibilty of axis labels, re-ordered certain figures for clarity, and several other small visual tweaks
</commit_message>
<xml_diff>
--- a/data/JeffCoCensus_Area_2020.xlsx
+++ b/data/JeffCoCensus_Area_2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b704ebb2f9605b8d/Desktop/JeffCo_Aquatic_Recreation_Survey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b704ebb2f9605b8d/Desktop/JeffCo_Aquatic_Recreation_Survey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64C8A6FA-5423-49E1-BC8D-5F26664DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{64C8A6FA-5423-49E1-BC8D-5F26664DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F68EAFB0-A25C-4B95-B7DE-7D943137EC9D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B709E725-B23E-470A-A3FC-0D6DBF99C0AF}"/>
   </bookViews>
@@ -463,6 +463,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>